<commit_message>
final push to git
</commit_message>
<xml_diff>
--- a/Excel Day2.xlsx
+++ b/Excel Day2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/srijan/Srijan/BBA Practical/Excel Sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{19866DE2-769E-CF4B-8311-7C4A5DF34BE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1C6A915-9937-A847-A44C-7774A75718DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="1800" windowWidth="28040" windowHeight="17440" activeTab="4" xr2:uid="{7A1DB880-16EA-0348-94B5-56B1E351D8C1}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="7" xr2:uid="{7A1DB880-16EA-0348-94B5-56B1E351D8C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Relative Referencing" sheetId="1" r:id="rId1"/>
@@ -18,11 +18,14 @@
     <sheet name="Mixed referencing" sheetId="3" r:id="rId3"/>
     <sheet name="Logical Functions" sheetId="4" r:id="rId4"/>
     <sheet name="Statistical Function" sheetId="5" r:id="rId5"/>
+    <sheet name="Marks Sheet" sheetId="6" r:id="rId6"/>
+    <sheet name="Marks Data" sheetId="7" r:id="rId7"/>
+    <sheet name="Mail merge data" sheetId="8" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Statistical Function'!$A$1:$F$151</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -42,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="108">
   <si>
     <t>Month</t>
   </si>
@@ -165,13 +168,214 @@
   </si>
   <si>
     <t>Iris-virginica</t>
+  </si>
+  <si>
+    <t>Roll No</t>
+  </si>
+  <si>
+    <t>SIDDHARTHA INTERNATIONAL COLLEGE</t>
+  </si>
+  <si>
+    <t>Affiliated to Pokhara Univeristy</t>
+  </si>
+  <si>
+    <t>SEMESTER EXAMINATION MARKS SHEET</t>
+  </si>
+  <si>
+    <t>Registration Number</t>
+  </si>
+  <si>
+    <t>Date of Birth</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Total Marks</t>
+  </si>
+  <si>
+    <t>TH</t>
+  </si>
+  <si>
+    <t>PR</t>
+  </si>
+  <si>
+    <t>Pass Marks</t>
+  </si>
+  <si>
+    <t>Marks Obtained</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>C Programming</t>
+  </si>
+  <si>
+    <t>Digital Logic</t>
+  </si>
+  <si>
+    <t>Mathematics I</t>
+  </si>
+  <si>
+    <t>Grade</t>
+  </si>
+  <si>
+    <t>Introduction to IT</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>First Semester</t>
+  </si>
+  <si>
+    <t>Full Name</t>
+  </si>
+  <si>
+    <t>C Programming (TH)</t>
+  </si>
+  <si>
+    <t>C Programming (PR)</t>
+  </si>
+  <si>
+    <t>Digital Logic (TH)</t>
+  </si>
+  <si>
+    <t>Digital Logic (PR)</t>
+  </si>
+  <si>
+    <t>Introduction to IT (TH)</t>
+  </si>
+  <si>
+    <t>Introduction to IT (PR)</t>
+  </si>
+  <si>
+    <t>Mathematics I (TH)</t>
+  </si>
+  <si>
+    <t>John Doe</t>
+  </si>
+  <si>
+    <t>Jane Smith</t>
+  </si>
+  <si>
+    <t>Robert Brown</t>
+  </si>
+  <si>
+    <t>Emily Johnson</t>
+  </si>
+  <si>
+    <t>Michael Davis</t>
+  </si>
+  <si>
+    <t>Jessica Wilson</t>
+  </si>
+  <si>
+    <t>David Anderson</t>
+  </si>
+  <si>
+    <t>Sarah Thomas</t>
+  </si>
+  <si>
+    <t>James Martinez</t>
+  </si>
+  <si>
+    <t>Linda Taylor</t>
+  </si>
+  <si>
+    <t>William Harris</t>
+  </si>
+  <si>
+    <t>Barbara Clark</t>
+  </si>
+  <si>
+    <t>Richard Lewis</t>
+  </si>
+  <si>
+    <t>Karen Walker</t>
+  </si>
+  <si>
+    <t>Joseph Hall</t>
+  </si>
+  <si>
+    <t>Patricia Allen</t>
+  </si>
+  <si>
+    <t>Thomas Young</t>
+  </si>
+  <si>
+    <t>Nancy King</t>
+  </si>
+  <si>
+    <t>Daniel Wright</t>
+  </si>
+  <si>
+    <t>Susan Scott</t>
+  </si>
+  <si>
+    <t>Matthew Green</t>
+  </si>
+  <si>
+    <t>Margaret Adams</t>
+  </si>
+  <si>
+    <t>Christopher Baker</t>
+  </si>
+  <si>
+    <t>Dorothy Nelson</t>
+  </si>
+  <si>
+    <t>Andrew Carter</t>
+  </si>
+  <si>
+    <t>A+</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B+</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Contact</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -214,8 +418,72 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="7" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="4" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="4" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -248,8 +516,38 @@
         <fgColor theme="8"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -287,6 +585,164 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -296,13 +752,14 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="5"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="4" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -312,7 +769,103 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="13" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="20% - Accent1" xfId="4" builtinId="30"/>
@@ -762,6 +1315,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
@@ -881,6 +1435,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -896,60 +1451,60 @@
   <sheetData>
     <row r="6" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B6" s="5"/>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B7" s="5"/>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="9" t="s">
         <v>25</v>
       </c>
       <c r="C8" s="5"/>
-      <c r="D8" s="9">
+      <c r="D8" s="6">
         <v>1</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8" s="6">
         <v>2</v>
       </c>
-      <c r="F8" s="9">
+      <c r="F8" s="6">
         <v>3</v>
       </c>
-      <c r="G8" s="9">
+      <c r="G8" s="6">
         <v>4</v>
       </c>
-      <c r="H8" s="9">
+      <c r="H8" s="6">
         <v>5</v>
       </c>
-      <c r="I8" s="9">
+      <c r="I8" s="6">
         <v>6</v>
       </c>
-      <c r="J8" s="9">
+      <c r="J8" s="6">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B9" s="8"/>
-      <c r="C9" s="9">
+      <c r="B9" s="9"/>
+      <c r="C9" s="6">
         <v>10</v>
       </c>
       <c r="D9" s="5"/>
@@ -961,8 +1516,8 @@
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B10" s="8"/>
-      <c r="C10" s="9">
+      <c r="B10" s="9"/>
+      <c r="C10" s="6">
         <v>20</v>
       </c>
       <c r="D10" s="5"/>
@@ -974,8 +1529,8 @@
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B11" s="8"/>
-      <c r="C11" s="9">
+      <c r="B11" s="9"/>
+      <c r="C11" s="6">
         <v>30</v>
       </c>
       <c r="D11" s="5"/>
@@ -987,8 +1542,8 @@
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B12" s="8"/>
-      <c r="C12" s="9">
+      <c r="B12" s="9"/>
+      <c r="C12" s="6">
         <v>40</v>
       </c>
       <c r="D12" s="5"/>
@@ -1000,8 +1555,8 @@
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B13" s="8"/>
-      <c r="C13" s="9">
+      <c r="B13" s="9"/>
+      <c r="C13" s="6">
         <v>50</v>
       </c>
       <c r="D13" s="5"/>
@@ -1065,6 +1620,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -1072,8 +1628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21C53F3D-43CD-5947-B0A8-896B41E99E1A}">
   <dimension ref="A1:F151"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="227" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView zoomScale="190" zoomScaleNormal="227" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4112,4 +4668,1326 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A782F6E-7DB4-4741-9F5C-A60C4582B7CD}">
+  <dimension ref="A1:O18"/>
+  <sheetViews>
+    <sheetView zoomScale="177" zoomScaleNormal="177" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.1640625" customWidth="1"/>
+    <col min="2" max="7" width="6.6640625" customWidth="1"/>
+    <col min="8" max="9" width="8.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="37">
+        <v>2025</v>
+      </c>
+      <c r="G1" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+    </row>
+    <row r="2" spans="1:15" ht="26" x14ac:dyDescent="0.3">
+      <c r="A2" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A3" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="40"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4" s="41" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="41"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="41"/>
+      <c r="H4" s="41"/>
+      <c r="I4" s="41"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A6" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="10">
+        <v>3</v>
+      </c>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="F6" s="18"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="10">
+        <f ca="1">LOOKUP(B6,'Marks Data'!A1:K26,'Marks Data'!B:B)</f>
+        <v>2025003</v>
+      </c>
+      <c r="I6" s="10"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A7" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="10" t="str">
+        <f>LOOKUP(B6,'Marks Data'!A1:K26,'Marks Data'!C1:C26)</f>
+        <v>Robert Brown</v>
+      </c>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="46">
+        <f>LOOKUP(B6,'Marks Data'!A1:K26,'Marks Data'!D1:D26)</f>
+        <v>38000</v>
+      </c>
+      <c r="I7" s="46"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A9" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="G9" s="15"/>
+      <c r="H9" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="I9" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="N9">
+        <v>40</v>
+      </c>
+      <c r="O9" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A10" s="20"/>
+      <c r="B10" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="G10" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22"/>
+      <c r="N10">
+        <v>50</v>
+      </c>
+      <c r="O10" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="N11">
+        <v>60</v>
+      </c>
+      <c r="O11" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5">
+        <v>32</v>
+      </c>
+      <c r="I12" s="5" t="str">
+        <f>VLOOKUP(H12,$N$8:$O$14,2,TRUE)</f>
+        <v>F</v>
+      </c>
+      <c r="N12">
+        <v>70</v>
+      </c>
+      <c r="O12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5">
+        <v>69</v>
+      </c>
+      <c r="I13" s="5" t="str">
+        <f>VLOOKUP(H13,$N$8:$O$14,2,TRUE)</f>
+        <v>B</v>
+      </c>
+      <c r="N13">
+        <v>80</v>
+      </c>
+      <c r="O13" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="N14">
+        <v>90</v>
+      </c>
+      <c r="O14" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+    </row>
+    <row r="16" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="11"/>
+      <c r="B16" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="25"/>
+      <c r="D16" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="E16" s="26"/>
+      <c r="F16" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="G16" s="28"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="12"/>
+      <c r="B17" s="29"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="33"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="13"/>
+      <c r="B18" s="34"/>
+      <c r="C18" s="35"/>
+      <c r="D18" s="34"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="G18" s="15"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="N8:O14">
+    <sortCondition ref="N14"/>
+  </sortState>
+  <mergeCells count="24">
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="D16:D18"/>
+    <mergeCell ref="C16:C18"/>
+    <mergeCell ref="E16:E18"/>
+    <mergeCell ref="F16:G17"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="H16:I17"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="A3:I3"/>
+    <mergeCell ref="A4:I4"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="F9:G9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C7367AC-BA85-BB43-83B0-37A7670F38EF}">
+  <dimension ref="A1:K40"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="42" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="42" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="42" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" s="42" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1" s="42" t="s">
+        <v>65</v>
+      </c>
+      <c r="I1" s="42" t="s">
+        <v>66</v>
+      </c>
+      <c r="J1" s="42" t="s">
+        <v>67</v>
+      </c>
+      <c r="K1" s="42" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="A2" s="43">
+        <v>1</v>
+      </c>
+      <c r="B2" s="43">
+        <v>2025001</v>
+      </c>
+      <c r="C2" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" s="44">
+        <v>38119</v>
+      </c>
+      <c r="E2" s="43">
+        <v>45</v>
+      </c>
+      <c r="F2" s="43">
+        <v>35</v>
+      </c>
+      <c r="G2" s="43">
+        <v>50</v>
+      </c>
+      <c r="H2" s="43">
+        <v>30</v>
+      </c>
+      <c r="I2" s="43">
+        <v>40</v>
+      </c>
+      <c r="J2" s="43">
+        <v>32</v>
+      </c>
+      <c r="K2" s="43">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="A3" s="43">
+        <v>2</v>
+      </c>
+      <c r="B3" s="43">
+        <v>2025002</v>
+      </c>
+      <c r="C3" s="43" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" s="44">
+        <v>37948</v>
+      </c>
+      <c r="E3" s="43">
+        <v>50</v>
+      </c>
+      <c r="F3" s="43">
+        <v>38</v>
+      </c>
+      <c r="G3" s="43">
+        <v>42</v>
+      </c>
+      <c r="H3" s="43">
+        <v>28</v>
+      </c>
+      <c r="I3" s="43">
+        <v>48</v>
+      </c>
+      <c r="J3" s="43">
+        <v>35</v>
+      </c>
+      <c r="K3" s="43">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="A4" s="43">
+        <v>3</v>
+      </c>
+      <c r="B4" s="43">
+        <v>2025003</v>
+      </c>
+      <c r="C4" s="43" t="s">
+        <v>71</v>
+      </c>
+      <c r="D4" s="44">
+        <v>38000</v>
+      </c>
+      <c r="E4" s="43">
+        <v>55</v>
+      </c>
+      <c r="F4" s="43">
+        <v>40</v>
+      </c>
+      <c r="G4" s="43">
+        <v>39</v>
+      </c>
+      <c r="H4" s="43">
+        <v>35</v>
+      </c>
+      <c r="I4" s="43">
+        <v>45</v>
+      </c>
+      <c r="J4" s="43">
+        <v>30</v>
+      </c>
+      <c r="K4" s="43">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="A5" s="43">
+        <v>4</v>
+      </c>
+      <c r="B5" s="43">
+        <v>2025004</v>
+      </c>
+      <c r="C5" s="43" t="s">
+        <v>72</v>
+      </c>
+      <c r="D5" s="44">
+        <v>37831</v>
+      </c>
+      <c r="E5" s="43">
+        <v>52</v>
+      </c>
+      <c r="F5" s="43">
+        <v>36</v>
+      </c>
+      <c r="G5" s="43">
+        <v>46</v>
+      </c>
+      <c r="H5" s="43">
+        <v>32</v>
+      </c>
+      <c r="I5" s="43">
+        <v>50</v>
+      </c>
+      <c r="J5" s="43">
+        <v>38</v>
+      </c>
+      <c r="K5" s="43">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="A6" s="43">
+        <v>5</v>
+      </c>
+      <c r="B6" s="43">
+        <v>2025005</v>
+      </c>
+      <c r="C6" s="43" t="s">
+        <v>73</v>
+      </c>
+      <c r="D6" s="44">
+        <v>38240</v>
+      </c>
+      <c r="E6" s="43">
+        <v>48</v>
+      </c>
+      <c r="F6" s="43">
+        <v>30</v>
+      </c>
+      <c r="G6" s="43">
+        <v>51</v>
+      </c>
+      <c r="H6" s="43">
+        <v>36</v>
+      </c>
+      <c r="I6" s="43">
+        <v>42</v>
+      </c>
+      <c r="J6" s="43">
+        <v>29</v>
+      </c>
+      <c r="K6" s="43">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="A7" s="43">
+        <v>6</v>
+      </c>
+      <c r="B7" s="43">
+        <v>2025006</v>
+      </c>
+      <c r="C7" s="43" t="s">
+        <v>74</v>
+      </c>
+      <c r="D7" s="44">
+        <v>37701</v>
+      </c>
+      <c r="E7" s="43">
+        <v>54</v>
+      </c>
+      <c r="F7" s="43">
+        <v>39</v>
+      </c>
+      <c r="G7" s="43">
+        <v>47</v>
+      </c>
+      <c r="H7" s="43">
+        <v>33</v>
+      </c>
+      <c r="I7" s="43">
+        <v>49</v>
+      </c>
+      <c r="J7" s="43">
+        <v>37</v>
+      </c>
+      <c r="K7" s="43">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="A8" s="43">
+        <v>7</v>
+      </c>
+      <c r="B8" s="43">
+        <v>2025007</v>
+      </c>
+      <c r="C8" s="43" t="s">
+        <v>75</v>
+      </c>
+      <c r="D8" s="44">
+        <v>38143</v>
+      </c>
+      <c r="E8" s="43">
+        <v>40</v>
+      </c>
+      <c r="F8" s="43">
+        <v>28</v>
+      </c>
+      <c r="G8" s="43">
+        <v>45</v>
+      </c>
+      <c r="H8" s="43">
+        <v>30</v>
+      </c>
+      <c r="I8" s="43">
+        <v>44</v>
+      </c>
+      <c r="J8" s="43">
+        <v>31</v>
+      </c>
+      <c r="K8" s="43">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="A9" s="43">
+        <v>8</v>
+      </c>
+      <c r="B9" s="43">
+        <v>2025008</v>
+      </c>
+      <c r="C9" s="43" t="s">
+        <v>76</v>
+      </c>
+      <c r="D9" s="44">
+        <v>37850</v>
+      </c>
+      <c r="E9" s="43">
+        <v>49</v>
+      </c>
+      <c r="F9" s="43">
+        <v>35</v>
+      </c>
+      <c r="G9" s="43">
+        <v>50</v>
+      </c>
+      <c r="H9" s="43">
+        <v>34</v>
+      </c>
+      <c r="I9" s="43">
+        <v>47</v>
+      </c>
+      <c r="J9" s="43">
+        <v>36</v>
+      </c>
+      <c r="K9" s="43">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="A10" s="43">
+        <v>9</v>
+      </c>
+      <c r="B10" s="43">
+        <v>2025009</v>
+      </c>
+      <c r="C10" s="43" t="s">
+        <v>77</v>
+      </c>
+      <c r="D10" s="44">
+        <v>38351</v>
+      </c>
+      <c r="E10" s="43">
+        <v>53</v>
+      </c>
+      <c r="F10" s="43">
+        <v>38</v>
+      </c>
+      <c r="G10" s="43">
+        <v>48</v>
+      </c>
+      <c r="H10" s="43">
+        <v>32</v>
+      </c>
+      <c r="I10" s="43">
+        <v>46</v>
+      </c>
+      <c r="J10" s="43">
+        <v>34</v>
+      </c>
+      <c r="K10" s="43">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="A11" s="43">
+        <v>10</v>
+      </c>
+      <c r="B11" s="43">
+        <v>2025010</v>
+      </c>
+      <c r="C11" s="43" t="s">
+        <v>78</v>
+      </c>
+      <c r="D11" s="44">
+        <v>37750</v>
+      </c>
+      <c r="E11" s="43">
+        <v>51</v>
+      </c>
+      <c r="F11" s="43">
+        <v>34</v>
+      </c>
+      <c r="G11" s="43">
+        <v>44</v>
+      </c>
+      <c r="H11" s="43">
+        <v>31</v>
+      </c>
+      <c r="I11" s="43">
+        <v>41</v>
+      </c>
+      <c r="J11" s="43">
+        <v>29</v>
+      </c>
+      <c r="K11" s="43">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="A12" s="43">
+        <v>11</v>
+      </c>
+      <c r="B12" s="43">
+        <v>2025011</v>
+      </c>
+      <c r="C12" s="43" t="s">
+        <v>79</v>
+      </c>
+      <c r="D12" s="44">
+        <v>38045</v>
+      </c>
+      <c r="E12" s="43">
+        <v>47</v>
+      </c>
+      <c r="F12" s="43">
+        <v>32</v>
+      </c>
+      <c r="G12" s="43">
+        <v>49</v>
+      </c>
+      <c r="H12" s="43">
+        <v>36</v>
+      </c>
+      <c r="I12" s="43">
+        <v>43</v>
+      </c>
+      <c r="J12" s="43">
+        <v>30</v>
+      </c>
+      <c r="K12" s="43">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="A13" s="43">
+        <v>12</v>
+      </c>
+      <c r="B13" s="43">
+        <v>2025012</v>
+      </c>
+      <c r="C13" s="43" t="s">
+        <v>80</v>
+      </c>
+      <c r="D13" s="44">
+        <v>37877</v>
+      </c>
+      <c r="E13" s="43">
+        <v>55</v>
+      </c>
+      <c r="F13" s="43">
+        <v>40</v>
+      </c>
+      <c r="G13" s="43">
+        <v>52</v>
+      </c>
+      <c r="H13" s="43">
+        <v>37</v>
+      </c>
+      <c r="I13" s="43">
+        <v>50</v>
+      </c>
+      <c r="J13" s="43">
+        <v>38</v>
+      </c>
+      <c r="K13" s="43">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="A14" s="43">
+        <v>13</v>
+      </c>
+      <c r="B14" s="43">
+        <v>2025013</v>
+      </c>
+      <c r="C14" s="43" t="s">
+        <v>81</v>
+      </c>
+      <c r="D14" s="44">
+        <v>38187</v>
+      </c>
+      <c r="E14" s="43">
+        <v>42</v>
+      </c>
+      <c r="F14" s="43">
+        <v>30</v>
+      </c>
+      <c r="G14" s="43">
+        <v>41</v>
+      </c>
+      <c r="H14" s="43">
+        <v>28</v>
+      </c>
+      <c r="I14" s="43">
+        <v>38</v>
+      </c>
+      <c r="J14" s="43">
+        <v>27</v>
+      </c>
+      <c r="K14" s="43">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="A15" s="43">
+        <v>14</v>
+      </c>
+      <c r="B15" s="43">
+        <v>2025014</v>
+      </c>
+      <c r="C15" s="43" t="s">
+        <v>82</v>
+      </c>
+      <c r="D15" s="44">
+        <v>37718</v>
+      </c>
+      <c r="E15" s="43">
+        <v>50</v>
+      </c>
+      <c r="F15" s="43">
+        <v>36</v>
+      </c>
+      <c r="G15" s="43">
+        <v>53</v>
+      </c>
+      <c r="H15" s="43">
+        <v>39</v>
+      </c>
+      <c r="I15" s="43">
+        <v>49</v>
+      </c>
+      <c r="J15" s="43">
+        <v>35</v>
+      </c>
+      <c r="K15" s="43">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="A16" s="43">
+        <v>15</v>
+      </c>
+      <c r="B16" s="43">
+        <v>2025015</v>
+      </c>
+      <c r="C16" s="43" t="s">
+        <v>83</v>
+      </c>
+      <c r="D16" s="44">
+        <v>38285</v>
+      </c>
+      <c r="E16" s="43">
+        <v>46</v>
+      </c>
+      <c r="F16" s="43">
+        <v>31</v>
+      </c>
+      <c r="G16" s="43">
+        <v>40</v>
+      </c>
+      <c r="H16" s="43">
+        <v>27</v>
+      </c>
+      <c r="I16" s="43">
+        <v>42</v>
+      </c>
+      <c r="J16" s="43">
+        <v>30</v>
+      </c>
+      <c r="K16" s="43">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="A17" s="43">
+        <v>16</v>
+      </c>
+      <c r="B17" s="43">
+        <v>2025016</v>
+      </c>
+      <c r="C17" s="43" t="s">
+        <v>84</v>
+      </c>
+      <c r="D17" s="44">
+        <v>37955</v>
+      </c>
+      <c r="E17" s="43">
+        <v>55</v>
+      </c>
+      <c r="F17" s="43">
+        <v>40</v>
+      </c>
+      <c r="G17" s="43">
+        <v>45</v>
+      </c>
+      <c r="H17" s="43">
+        <v>31</v>
+      </c>
+      <c r="I17" s="43">
+        <v>51</v>
+      </c>
+      <c r="J17" s="43">
+        <v>37</v>
+      </c>
+      <c r="K17" s="43">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="A18" s="43">
+        <v>17</v>
+      </c>
+      <c r="B18" s="43">
+        <v>2025017</v>
+      </c>
+      <c r="C18" s="43" t="s">
+        <v>85</v>
+      </c>
+      <c r="D18" s="44">
+        <v>38061</v>
+      </c>
+      <c r="E18" s="43">
+        <v>48</v>
+      </c>
+      <c r="F18" s="43">
+        <v>33</v>
+      </c>
+      <c r="G18" s="43">
+        <v>47</v>
+      </c>
+      <c r="H18" s="43">
+        <v>34</v>
+      </c>
+      <c r="I18" s="43">
+        <v>44</v>
+      </c>
+      <c r="J18" s="43">
+        <v>32</v>
+      </c>
+      <c r="K18" s="43">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="A19" s="43">
+        <v>18</v>
+      </c>
+      <c r="B19" s="43">
+        <v>2025018</v>
+      </c>
+      <c r="C19" s="43" t="s">
+        <v>86</v>
+      </c>
+      <c r="D19" s="44">
+        <v>37799</v>
+      </c>
+      <c r="E19" s="43">
+        <v>52</v>
+      </c>
+      <c r="F19" s="43">
+        <v>38</v>
+      </c>
+      <c r="G19" s="43">
+        <v>50</v>
+      </c>
+      <c r="H19" s="43">
+        <v>36</v>
+      </c>
+      <c r="I19" s="43">
+        <v>48</v>
+      </c>
+      <c r="J19" s="43">
+        <v>35</v>
+      </c>
+      <c r="K19" s="43">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="A20" s="43">
+        <v>19</v>
+      </c>
+      <c r="B20" s="43">
+        <v>2025019</v>
+      </c>
+      <c r="C20" s="43" t="s">
+        <v>87</v>
+      </c>
+      <c r="D20" s="44">
+        <v>38210</v>
+      </c>
+      <c r="E20" s="43">
+        <v>45</v>
+      </c>
+      <c r="F20" s="43">
+        <v>29</v>
+      </c>
+      <c r="G20" s="43">
+        <v>39</v>
+      </c>
+      <c r="H20" s="43">
+        <v>25</v>
+      </c>
+      <c r="I20" s="43">
+        <v>37</v>
+      </c>
+      <c r="J20" s="43">
+        <v>26</v>
+      </c>
+      <c r="K20" s="43">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="A21" s="43">
+        <v>20</v>
+      </c>
+      <c r="B21" s="43">
+        <v>2025020</v>
+      </c>
+      <c r="C21" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="D21" s="44">
+        <v>37916</v>
+      </c>
+      <c r="E21" s="43">
+        <v>49</v>
+      </c>
+      <c r="F21" s="43">
+        <v>35</v>
+      </c>
+      <c r="G21" s="43">
+        <v>43</v>
+      </c>
+      <c r="H21" s="43">
+        <v>30</v>
+      </c>
+      <c r="I21" s="43">
+        <v>41</v>
+      </c>
+      <c r="J21" s="43">
+        <v>28</v>
+      </c>
+      <c r="K21" s="43">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="A22" s="43">
+        <v>21</v>
+      </c>
+      <c r="B22" s="43">
+        <v>2025021</v>
+      </c>
+      <c r="C22" s="43" t="s">
+        <v>89</v>
+      </c>
+      <c r="D22" s="44">
+        <v>37994</v>
+      </c>
+      <c r="E22" s="43">
+        <v>53</v>
+      </c>
+      <c r="F22" s="43">
+        <v>39</v>
+      </c>
+      <c r="G22" s="43">
+        <v>48</v>
+      </c>
+      <c r="H22" s="43">
+        <v>34</v>
+      </c>
+      <c r="I22" s="43">
+        <v>46</v>
+      </c>
+      <c r="J22" s="43">
+        <v>33</v>
+      </c>
+      <c r="K22" s="43">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="A23" s="43">
+        <v>22</v>
+      </c>
+      <c r="B23" s="43">
+        <v>2025022</v>
+      </c>
+      <c r="C23" s="43" t="s">
+        <v>90</v>
+      </c>
+      <c r="D23" s="44">
+        <v>37807</v>
+      </c>
+      <c r="E23" s="43">
+        <v>44</v>
+      </c>
+      <c r="F23" s="43">
+        <v>28</v>
+      </c>
+      <c r="G23" s="43">
+        <v>42</v>
+      </c>
+      <c r="H23" s="43">
+        <v>29</v>
+      </c>
+      <c r="I23" s="43">
+        <v>40</v>
+      </c>
+      <c r="J23" s="43">
+        <v>27</v>
+      </c>
+      <c r="K23" s="43">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="A24" s="43">
+        <v>23</v>
+      </c>
+      <c r="B24" s="43">
+        <v>2025023</v>
+      </c>
+      <c r="C24" s="43" t="s">
+        <v>91</v>
+      </c>
+      <c r="D24" s="44">
+        <v>38244</v>
+      </c>
+      <c r="E24" s="43">
+        <v>51</v>
+      </c>
+      <c r="F24" s="43">
+        <v>37</v>
+      </c>
+      <c r="G24" s="43">
+        <v>49</v>
+      </c>
+      <c r="H24" s="43">
+        <v>35</v>
+      </c>
+      <c r="I24" s="43">
+        <v>45</v>
+      </c>
+      <c r="J24" s="43">
+        <v>31</v>
+      </c>
+      <c r="K24" s="43">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="A25" s="43">
+        <v>24</v>
+      </c>
+      <c r="B25" s="43">
+        <v>2025024</v>
+      </c>
+      <c r="C25" s="43" t="s">
+        <v>92</v>
+      </c>
+      <c r="D25" s="44">
+        <v>37670</v>
+      </c>
+      <c r="E25" s="43">
+        <v>47</v>
+      </c>
+      <c r="F25" s="43">
+        <v>32</v>
+      </c>
+      <c r="G25" s="43">
+        <v>44</v>
+      </c>
+      <c r="H25" s="43">
+        <v>30</v>
+      </c>
+      <c r="I25" s="43">
+        <v>42</v>
+      </c>
+      <c r="J25" s="43">
+        <v>28</v>
+      </c>
+      <c r="K25" s="43">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="A26" s="43">
+        <v>25</v>
+      </c>
+      <c r="B26" s="43">
+        <v>2025025</v>
+      </c>
+      <c r="C26" s="43" t="s">
+        <v>93</v>
+      </c>
+      <c r="D26" s="44">
+        <v>38127</v>
+      </c>
+      <c r="E26" s="43">
+        <v>55</v>
+      </c>
+      <c r="F26" s="43">
+        <v>40</v>
+      </c>
+      <c r="G26" s="43">
+        <v>50</v>
+      </c>
+      <c r="H26" s="43">
+        <v>38</v>
+      </c>
+      <c r="I26" s="43">
+        <v>48</v>
+      </c>
+      <c r="J26" s="43">
+        <v>36</v>
+      </c>
+      <c r="K26" s="43">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="39" spans="6:6" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="6:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F40" s="45"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9168643-8BDD-C042-A253-07F55D140D55}">
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26" customWidth="1"/>
+    <col min="7" max="7" width="16.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="48" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="47" t="s">
+        <v>102</v>
+      </c>
+      <c r="B1" s="47" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1" s="47" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1" s="47" t="s">
+        <v>104</v>
+      </c>
+      <c r="E1" s="47" t="s">
+        <v>105</v>
+      </c>
+      <c r="F1" s="47" t="s">
+        <v>106</v>
+      </c>
+      <c r="G1" s="47" t="s">
+        <v>107</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>